<commit_message>
delnat and bozinovic data extraction for acclimation analysis
</commit_message>
<xml_diff>
--- a/data extraction /extraction /acclimation /data/acclimation_full_2june21.xlsx
+++ b/data extraction /extraction /acclimation /data/acclimation_full_2june21.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /extraction /acclimation /data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C889B0-0BFB-C94D-96A2-ACE79101E703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5939005-3CB2-B340-8E0B-B44033AC5809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16180" windowHeight="16060" xr2:uid="{BC548A7C-C40E-CC48-BA60-2918C3D37144}"/>
+    <workbookView xWindow="29360" yWindow="-16960" windowWidth="23500" windowHeight="12900" xr2:uid="{BC548A7C-C40E-CC48-BA60-2918C3D37144}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1800" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1930" uniqueCount="126">
   <si>
     <t>response_id</t>
   </si>
@@ -364,6 +364,45 @@
   </si>
   <si>
     <t>cf. folsomi</t>
+  </si>
+  <si>
+    <t>bozinovic2016</t>
+  </si>
+  <si>
+    <t>Scope of thermal tolerance (CTmax - CTmin)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drosophila </t>
+  </si>
+  <si>
+    <t>melanogaster</t>
+  </si>
+  <si>
+    <t>delnat2019</t>
+  </si>
+  <si>
+    <t>Culex</t>
+  </si>
+  <si>
+    <t>pipiens</t>
+  </si>
+  <si>
+    <t>insecticide exposure</t>
+  </si>
+  <si>
+    <t>absence</t>
+  </si>
+  <si>
+    <t>presence</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
   </si>
 </sst>
 </file>
@@ -730,11 +769,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FD9C74-7293-0D4C-AEEE-5123D41AED94}">
-  <dimension ref="A1:AH288"/>
+  <dimension ref="A1:AH303"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A263" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R289" sqref="R289"/>
+      <pane ySplit="1" topLeftCell="A285" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M302" sqref="M302:M303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22804,6 +22843,1236 @@
         <v>1</v>
       </c>
     </row>
+    <row r="289" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A289" s="1">
+        <v>1</v>
+      </c>
+      <c r="B289" s="1">
+        <v>1</v>
+      </c>
+      <c r="C289" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D289" t="s">
+        <v>74</v>
+      </c>
+      <c r="E289" s="1">
+        <v>0</v>
+      </c>
+      <c r="F289" s="1">
+        <v>1</v>
+      </c>
+      <c r="H289" s="1">
+        <v>20</v>
+      </c>
+      <c r="I289" s="1">
+        <v>10</v>
+      </c>
+      <c r="J289">
+        <v>24</v>
+      </c>
+      <c r="K289" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L289" t="s">
+        <v>43</v>
+      </c>
+      <c r="M289">
+        <v>7.9081911772020703</v>
+      </c>
+      <c r="N289">
+        <v>8.4562590142737406</v>
+      </c>
+      <c r="O289">
+        <v>0.28845675635350965</v>
+      </c>
+      <c r="P289">
+        <v>0.28845675635350965</v>
+      </c>
+      <c r="Q289" s="1">
+        <v>200</v>
+      </c>
+      <c r="R289" s="1">
+        <v>200</v>
+      </c>
+      <c r="S289" s="1">
+        <v>1</v>
+      </c>
+      <c r="T289" s="1">
+        <v>1</v>
+      </c>
+      <c r="U289" t="s">
+        <v>115</v>
+      </c>
+      <c r="V289" t="s">
+        <v>116</v>
+      </c>
+      <c r="W289" s="1">
+        <v>1</v>
+      </c>
+      <c r="X289" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y289" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A290" s="1">
+        <v>2</v>
+      </c>
+      <c r="B290" s="1">
+        <v>1</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D290" t="s">
+        <v>74</v>
+      </c>
+      <c r="E290" s="1">
+        <v>0</v>
+      </c>
+      <c r="F290" s="1">
+        <v>1</v>
+      </c>
+      <c r="H290" s="1">
+        <v>20</v>
+      </c>
+      <c r="I290" s="1">
+        <v>10</v>
+      </c>
+      <c r="J290">
+        <v>24</v>
+      </c>
+      <c r="K290" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L290" t="s">
+        <v>43</v>
+      </c>
+      <c r="M290" s="3">
+        <v>37.837965140000001</v>
+      </c>
+      <c r="N290">
+        <v>38.114178049929301</v>
+      </c>
+      <c r="O290">
+        <v>0.21818181818180449</v>
+      </c>
+      <c r="P290">
+        <v>0.21818181818179738</v>
+      </c>
+      <c r="Q290" s="1">
+        <v>200</v>
+      </c>
+      <c r="R290" s="1">
+        <v>200</v>
+      </c>
+      <c r="S290" s="1">
+        <v>1</v>
+      </c>
+      <c r="T290" s="1">
+        <v>1</v>
+      </c>
+      <c r="U290" t="s">
+        <v>115</v>
+      </c>
+      <c r="V290" t="s">
+        <v>116</v>
+      </c>
+      <c r="W290" s="1">
+        <v>1</v>
+      </c>
+      <c r="X290" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y290" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="291" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A291" s="1">
+        <v>1</v>
+      </c>
+      <c r="B291" s="1">
+        <v>2</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D291" t="s">
+        <v>80</v>
+      </c>
+      <c r="E291" s="1">
+        <v>0</v>
+      </c>
+      <c r="F291" s="1">
+        <v>1</v>
+      </c>
+      <c r="H291" s="1">
+        <v>20</v>
+      </c>
+      <c r="I291" s="1">
+        <v>10</v>
+      </c>
+      <c r="J291">
+        <v>24</v>
+      </c>
+      <c r="K291" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="L291" t="s">
+        <v>43</v>
+      </c>
+      <c r="M291">
+        <v>29.868428605139101</v>
+      </c>
+      <c r="N291">
+        <v>29.594316217784701</v>
+      </c>
+      <c r="O291">
+        <v>0.24911190902889757</v>
+      </c>
+      <c r="P291">
+        <v>0.24911190902889757</v>
+      </c>
+      <c r="Q291" s="1">
+        <v>200</v>
+      </c>
+      <c r="R291" s="1">
+        <v>200</v>
+      </c>
+      <c r="S291" s="1">
+        <v>1</v>
+      </c>
+      <c r="T291" s="1">
+        <v>1</v>
+      </c>
+      <c r="U291" t="s">
+        <v>115</v>
+      </c>
+      <c r="V291" t="s">
+        <v>116</v>
+      </c>
+      <c r="W291" s="1">
+        <v>1</v>
+      </c>
+      <c r="X291" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y291" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="292" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A292" s="1">
+        <v>1</v>
+      </c>
+      <c r="B292" s="1">
+        <v>1</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D292" t="s">
+        <v>51</v>
+      </c>
+      <c r="E292" s="1">
+        <v>0</v>
+      </c>
+      <c r="F292" s="1">
+        <v>1</v>
+      </c>
+      <c r="H292" s="1">
+        <v>20</v>
+      </c>
+      <c r="I292" s="1">
+        <v>7</v>
+      </c>
+      <c r="J292">
+        <v>24</v>
+      </c>
+      <c r="K292" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L292" t="s">
+        <v>43</v>
+      </c>
+      <c r="M292">
+        <v>40.6</v>
+      </c>
+      <c r="N292">
+        <v>40.864150943396197</v>
+      </c>
+      <c r="O292">
+        <v>0.30377358490564887</v>
+      </c>
+      <c r="P292">
+        <v>0.30377358490570217</v>
+      </c>
+      <c r="Q292" s="1">
+        <v>75</v>
+      </c>
+      <c r="R292" s="1">
+        <v>78</v>
+      </c>
+      <c r="S292" s="1">
+        <v>1</v>
+      </c>
+      <c r="T292" s="1">
+        <v>0</v>
+      </c>
+      <c r="U292" t="s">
+        <v>118</v>
+      </c>
+      <c r="V292" t="s">
+        <v>119</v>
+      </c>
+      <c r="W292" s="1">
+        <v>1</v>
+      </c>
+      <c r="X292" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y292" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z292" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA292" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="293" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A293" s="1">
+        <v>1</v>
+      </c>
+      <c r="B293" s="1">
+        <v>1</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D293" t="s">
+        <v>51</v>
+      </c>
+      <c r="E293" s="1">
+        <v>0</v>
+      </c>
+      <c r="F293" s="1">
+        <v>1</v>
+      </c>
+      <c r="H293" s="1">
+        <v>20</v>
+      </c>
+      <c r="I293" s="1">
+        <v>7</v>
+      </c>
+      <c r="J293">
+        <v>24</v>
+      </c>
+      <c r="K293" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L293" t="s">
+        <v>43</v>
+      </c>
+      <c r="M293">
+        <v>36.796226415094303</v>
+      </c>
+      <c r="N293">
+        <v>35.9509433962264</v>
+      </c>
+      <c r="O293">
+        <v>0.30377358490569861</v>
+      </c>
+      <c r="P293">
+        <v>0.31698113207544765</v>
+      </c>
+      <c r="Q293" s="1">
+        <v>78</v>
+      </c>
+      <c r="R293" s="1">
+        <v>76</v>
+      </c>
+      <c r="S293" s="1">
+        <v>1</v>
+      </c>
+      <c r="T293" s="1">
+        <v>0</v>
+      </c>
+      <c r="U293" t="s">
+        <v>118</v>
+      </c>
+      <c r="V293" t="s">
+        <v>119</v>
+      </c>
+      <c r="W293" s="1">
+        <v>1</v>
+      </c>
+      <c r="X293" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y293" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z293" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA293" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="294" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A294" s="1">
+        <v>1</v>
+      </c>
+      <c r="B294" s="1">
+        <v>1</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D294" t="s">
+        <v>51</v>
+      </c>
+      <c r="E294" s="1">
+        <v>0</v>
+      </c>
+      <c r="F294" s="1">
+        <v>1</v>
+      </c>
+      <c r="H294" s="1">
+        <v>20</v>
+      </c>
+      <c r="I294" s="1">
+        <v>14</v>
+      </c>
+      <c r="J294">
+        <v>24</v>
+      </c>
+      <c r="K294" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L294" t="s">
+        <v>43</v>
+      </c>
+      <c r="M294">
+        <v>40.6</v>
+      </c>
+      <c r="N294">
+        <v>41.022641509433903</v>
+      </c>
+      <c r="O294">
+        <v>0.30377358490564887</v>
+      </c>
+      <c r="P294">
+        <v>0.31698113207550094</v>
+      </c>
+      <c r="Q294" s="1">
+        <v>75</v>
+      </c>
+      <c r="R294" s="1">
+        <v>72</v>
+      </c>
+      <c r="S294" s="1">
+        <v>1</v>
+      </c>
+      <c r="T294" s="1">
+        <v>0</v>
+      </c>
+      <c r="U294" t="s">
+        <v>118</v>
+      </c>
+      <c r="V294" t="s">
+        <v>119</v>
+      </c>
+      <c r="W294" s="1">
+        <v>1</v>
+      </c>
+      <c r="X294" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y294" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z294" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA294" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="295" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A295" s="1">
+        <v>1</v>
+      </c>
+      <c r="B295" s="1">
+        <v>1</v>
+      </c>
+      <c r="C295" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D295" t="s">
+        <v>51</v>
+      </c>
+      <c r="E295" s="1">
+        <v>0</v>
+      </c>
+      <c r="F295" s="1">
+        <v>1</v>
+      </c>
+      <c r="H295" s="1">
+        <v>20</v>
+      </c>
+      <c r="I295" s="1">
+        <v>14</v>
+      </c>
+      <c r="J295">
+        <v>24</v>
+      </c>
+      <c r="K295" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L295" t="s">
+        <v>43</v>
+      </c>
+      <c r="M295">
+        <v>36.796226415094303</v>
+      </c>
+      <c r="N295">
+        <v>38.090566037735798</v>
+      </c>
+      <c r="O295">
+        <v>0.30377358490569861</v>
+      </c>
+      <c r="P295">
+        <v>0.34339622641509848</v>
+      </c>
+      <c r="Q295" s="1">
+        <v>78</v>
+      </c>
+      <c r="R295" s="1">
+        <v>68</v>
+      </c>
+      <c r="S295" s="1">
+        <v>1</v>
+      </c>
+      <c r="T295" s="1">
+        <v>0</v>
+      </c>
+      <c r="U295" t="s">
+        <v>118</v>
+      </c>
+      <c r="V295" t="s">
+        <v>119</v>
+      </c>
+      <c r="W295" s="1">
+        <v>1</v>
+      </c>
+      <c r="X295" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y295" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z295" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA295" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="296" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A296" s="1">
+        <v>1</v>
+      </c>
+      <c r="B296" s="1">
+        <v>2</v>
+      </c>
+      <c r="C296" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D296" t="s">
+        <v>53</v>
+      </c>
+      <c r="E296" s="1">
+        <v>0</v>
+      </c>
+      <c r="F296" s="1">
+        <v>1</v>
+      </c>
+      <c r="H296" s="1">
+        <v>20</v>
+      </c>
+      <c r="I296" s="1">
+        <v>7</v>
+      </c>
+      <c r="J296">
+        <v>24</v>
+      </c>
+      <c r="K296" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L296" t="s">
+        <v>43</v>
+      </c>
+      <c r="M296">
+        <v>39.411320754716897</v>
+      </c>
+      <c r="N296">
+        <v>40.098113207547101</v>
+      </c>
+      <c r="O296">
+        <v>0.27735849056604778</v>
+      </c>
+      <c r="P296">
+        <v>0.33018867924524997</v>
+      </c>
+      <c r="Q296" s="1">
+        <v>106</v>
+      </c>
+      <c r="R296" s="1">
+        <v>76</v>
+      </c>
+      <c r="S296" s="1">
+        <v>1</v>
+      </c>
+      <c r="T296" s="1">
+        <v>0</v>
+      </c>
+      <c r="U296" t="s">
+        <v>118</v>
+      </c>
+      <c r="V296" t="s">
+        <v>119</v>
+      </c>
+      <c r="W296" s="1">
+        <v>1</v>
+      </c>
+      <c r="X296" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y296" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z296" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA296" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB296" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC296" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="297" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A297" s="1">
+        <v>1</v>
+      </c>
+      <c r="B297" s="1">
+        <v>2</v>
+      </c>
+      <c r="C297" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D297" t="s">
+        <v>53</v>
+      </c>
+      <c r="E297" s="1">
+        <v>0</v>
+      </c>
+      <c r="F297" s="1">
+        <v>1</v>
+      </c>
+      <c r="H297" s="1">
+        <v>20</v>
+      </c>
+      <c r="I297" s="1">
+        <v>7</v>
+      </c>
+      <c r="J297">
+        <v>24</v>
+      </c>
+      <c r="K297" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L297" t="s">
+        <v>43</v>
+      </c>
+      <c r="M297">
+        <v>36.2415094339622</v>
+      </c>
+      <c r="N297">
+        <v>37.7735849056603</v>
+      </c>
+      <c r="O297">
+        <v>0.40943396226414919</v>
+      </c>
+      <c r="P297">
+        <v>0.36981132075474932</v>
+      </c>
+      <c r="Q297" s="1">
+        <v>50</v>
+      </c>
+      <c r="R297" s="1">
+        <v>60</v>
+      </c>
+      <c r="S297" s="1">
+        <v>1</v>
+      </c>
+      <c r="T297" s="1">
+        <v>0</v>
+      </c>
+      <c r="U297" t="s">
+        <v>118</v>
+      </c>
+      <c r="V297" t="s">
+        <v>119</v>
+      </c>
+      <c r="W297" s="1">
+        <v>1</v>
+      </c>
+      <c r="X297" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y297" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z297" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA297" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB297" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC297" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="298" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A298" s="1">
+        <v>1</v>
+      </c>
+      <c r="B298" s="1">
+        <v>2</v>
+      </c>
+      <c r="C298" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D298" t="s">
+        <v>53</v>
+      </c>
+      <c r="E298" s="1">
+        <v>0</v>
+      </c>
+      <c r="F298" s="1">
+        <v>1</v>
+      </c>
+      <c r="H298" s="1">
+        <v>20</v>
+      </c>
+      <c r="I298" s="1">
+        <v>14</v>
+      </c>
+      <c r="J298">
+        <v>24</v>
+      </c>
+      <c r="K298" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L298" t="s">
+        <v>43</v>
+      </c>
+      <c r="M298">
+        <v>39.411320754716897</v>
+      </c>
+      <c r="N298">
+        <v>40.071698113207503</v>
+      </c>
+      <c r="O298">
+        <v>0.27735849056604778</v>
+      </c>
+      <c r="P298">
+        <v>0.30377358490564887</v>
+      </c>
+      <c r="Q298" s="1">
+        <v>106</v>
+      </c>
+      <c r="R298" s="1">
+        <v>89</v>
+      </c>
+      <c r="S298" s="1">
+        <v>1</v>
+      </c>
+      <c r="T298" s="1">
+        <v>0</v>
+      </c>
+      <c r="U298" t="s">
+        <v>118</v>
+      </c>
+      <c r="V298" t="s">
+        <v>119</v>
+      </c>
+      <c r="W298" s="1">
+        <v>1</v>
+      </c>
+      <c r="X298" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y298" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z298" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA298" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB298" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC298" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="299" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A299" s="1">
+        <v>1</v>
+      </c>
+      <c r="B299" s="1">
+        <v>2</v>
+      </c>
+      <c r="C299" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D299" t="s">
+        <v>53</v>
+      </c>
+      <c r="E299" s="1">
+        <v>0</v>
+      </c>
+      <c r="F299" s="1">
+        <v>1</v>
+      </c>
+      <c r="H299" s="1">
+        <v>20</v>
+      </c>
+      <c r="I299" s="1">
+        <v>14</v>
+      </c>
+      <c r="J299">
+        <v>24</v>
+      </c>
+      <c r="K299" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L299" t="s">
+        <v>43</v>
+      </c>
+      <c r="M299">
+        <v>36.2415094339622</v>
+      </c>
+      <c r="N299">
+        <v>37.562264150943399</v>
+      </c>
+      <c r="O299">
+        <v>0.40943396226414919</v>
+      </c>
+      <c r="P299">
+        <v>0.44905660377354906</v>
+      </c>
+      <c r="Q299" s="1">
+        <v>50</v>
+      </c>
+      <c r="R299" s="1">
+        <v>44</v>
+      </c>
+      <c r="S299" s="1">
+        <v>1</v>
+      </c>
+      <c r="T299" s="1">
+        <v>0</v>
+      </c>
+      <c r="U299" t="s">
+        <v>118</v>
+      </c>
+      <c r="V299" t="s">
+        <v>119</v>
+      </c>
+      <c r="W299" s="1">
+        <v>1</v>
+      </c>
+      <c r="X299" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y299" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z299" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA299" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB299" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC299" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="300" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A300" s="1">
+        <v>1</v>
+      </c>
+      <c r="B300" s="1">
+        <v>3</v>
+      </c>
+      <c r="C300" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D300" t="s">
+        <v>54</v>
+      </c>
+      <c r="E300" s="1">
+        <v>0</v>
+      </c>
+      <c r="F300" s="1">
+        <v>1</v>
+      </c>
+      <c r="H300" s="1">
+        <v>20</v>
+      </c>
+      <c r="I300" s="1">
+        <v>14</v>
+      </c>
+      <c r="J300">
+        <v>24</v>
+      </c>
+      <c r="K300" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L300" t="s">
+        <v>43</v>
+      </c>
+      <c r="M300">
+        <v>40.018867924528301</v>
+      </c>
+      <c r="N300">
+        <v>40.784905660377298</v>
+      </c>
+      <c r="O300">
+        <v>0.36981132075474932</v>
+      </c>
+      <c r="P300">
+        <v>0.39622641509435041</v>
+      </c>
+      <c r="Q300" s="1">
+        <v>84</v>
+      </c>
+      <c r="R300" s="1">
+        <v>63</v>
+      </c>
+      <c r="S300" s="1">
+        <v>1</v>
+      </c>
+      <c r="T300" s="1">
+        <v>0</v>
+      </c>
+      <c r="U300" t="s">
+        <v>118</v>
+      </c>
+      <c r="V300" t="s">
+        <v>119</v>
+      </c>
+      <c r="W300" s="1">
+        <v>1</v>
+      </c>
+      <c r="X300" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y300" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z300" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA300" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB300" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC300" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="301" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A301" s="1">
+        <v>1</v>
+      </c>
+      <c r="B301" s="1">
+        <v>3</v>
+      </c>
+      <c r="C301" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D301" t="s">
+        <v>54</v>
+      </c>
+      <c r="E301" s="1">
+        <v>0</v>
+      </c>
+      <c r="F301" s="1">
+        <v>1</v>
+      </c>
+      <c r="H301" s="1">
+        <v>20</v>
+      </c>
+      <c r="I301" s="1">
+        <v>14</v>
+      </c>
+      <c r="J301">
+        <v>24</v>
+      </c>
+      <c r="K301" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L301" t="s">
+        <v>43</v>
+      </c>
+      <c r="M301">
+        <v>39.543396226415098</v>
+      </c>
+      <c r="N301">
+        <v>38.539622641509403</v>
+      </c>
+      <c r="O301">
+        <v>0.38301886792454809</v>
+      </c>
+      <c r="P301">
+        <v>0.39622641509435041</v>
+      </c>
+      <c r="Q301" s="1">
+        <v>68</v>
+      </c>
+      <c r="R301" s="1">
+        <v>60</v>
+      </c>
+      <c r="S301" s="1">
+        <v>1</v>
+      </c>
+      <c r="T301" s="1">
+        <v>0</v>
+      </c>
+      <c r="U301" t="s">
+        <v>118</v>
+      </c>
+      <c r="V301" t="s">
+        <v>119</v>
+      </c>
+      <c r="W301" s="1">
+        <v>1</v>
+      </c>
+      <c r="X301" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y301" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z301" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA301" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB301" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC301" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="302" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A302" s="1">
+        <v>1</v>
+      </c>
+      <c r="B302" s="1">
+        <v>3</v>
+      </c>
+      <c r="C302" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D302" t="s">
+        <v>54</v>
+      </c>
+      <c r="E302" s="1">
+        <v>0</v>
+      </c>
+      <c r="F302" s="1">
+        <v>1</v>
+      </c>
+      <c r="H302" s="1">
+        <v>20</v>
+      </c>
+      <c r="I302" s="1">
+        <v>14</v>
+      </c>
+      <c r="J302">
+        <v>24</v>
+      </c>
+      <c r="K302" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L302" t="s">
+        <v>43</v>
+      </c>
+      <c r="M302">
+        <v>40.018867924528301</v>
+      </c>
+      <c r="N302">
+        <v>41.075471698113198</v>
+      </c>
+      <c r="O302">
+        <v>0.36981132075474932</v>
+      </c>
+      <c r="P302">
+        <v>0.42264150943395151</v>
+      </c>
+      <c r="Q302" s="1">
+        <v>84</v>
+      </c>
+      <c r="R302" s="1">
+        <v>57</v>
+      </c>
+      <c r="S302" s="1">
+        <v>1</v>
+      </c>
+      <c r="T302" s="1">
+        <v>0</v>
+      </c>
+      <c r="U302" t="s">
+        <v>118</v>
+      </c>
+      <c r="V302" t="s">
+        <v>119</v>
+      </c>
+      <c r="W302" s="1">
+        <v>1</v>
+      </c>
+      <c r="X302" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y302" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z302" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA302" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB302" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC302" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="303" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A303" s="1">
+        <v>1</v>
+      </c>
+      <c r="B303" s="1">
+        <v>3</v>
+      </c>
+      <c r="C303" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D303" t="s">
+        <v>54</v>
+      </c>
+      <c r="E303" s="1">
+        <v>0</v>
+      </c>
+      <c r="F303" s="1">
+        <v>1</v>
+      </c>
+      <c r="H303" s="1">
+        <v>20</v>
+      </c>
+      <c r="I303" s="1">
+        <v>14</v>
+      </c>
+      <c r="J303">
+        <v>24</v>
+      </c>
+      <c r="K303" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L303" t="s">
+        <v>43</v>
+      </c>
+      <c r="M303">
+        <v>39.543396226415098</v>
+      </c>
+      <c r="N303">
+        <v>38.803773584905599</v>
+      </c>
+      <c r="O303">
+        <v>0.38301886792454809</v>
+      </c>
+      <c r="P303">
+        <v>0.38301886792455164</v>
+      </c>
+      <c r="Q303" s="1">
+        <v>68</v>
+      </c>
+      <c r="R303" s="1">
+        <v>65</v>
+      </c>
+      <c r="S303" s="1">
+        <v>1</v>
+      </c>
+      <c r="T303" s="1">
+        <v>0</v>
+      </c>
+      <c r="U303" t="s">
+        <v>118</v>
+      </c>
+      <c r="V303" t="s">
+        <v>119</v>
+      </c>
+      <c r="W303" s="1">
+        <v>1</v>
+      </c>
+      <c r="X303" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y303" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z303" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA303" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB303" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC303" t="s">
+        <v>125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
haupt et al 2017 data extraction
</commit_message>
<xml_diff>
--- a/data extraction /extraction /acclimation /data/acclimation_full_2june21.xlsx
+++ b/data extraction /extraction /acclimation /data/acclimation_full_2june21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /extraction /acclimation /data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5939005-3CB2-B340-8E0B-B44033AC5809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60ADDCA2-C131-8146-958B-C81FB0CCCB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29360" yWindow="-16960" windowWidth="23500" windowHeight="12900" xr2:uid="{BC548A7C-C40E-CC48-BA60-2918C3D37144}"/>
+    <workbookView xWindow="29420" yWindow="-24160" windowWidth="23500" windowHeight="12900" xr2:uid="{BC548A7C-C40E-CC48-BA60-2918C3D37144}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1930" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2024" uniqueCount="139">
   <si>
     <t>response_id</t>
   </si>
@@ -404,6 +404,45 @@
   <si>
     <t>female</t>
   </si>
+  <si>
+    <t>haupt2017</t>
+  </si>
+  <si>
+    <t>Tpref</t>
+  </si>
+  <si>
+    <t>Topt</t>
+  </si>
+  <si>
+    <t>Table 2</t>
+  </si>
+  <si>
+    <t>mm * sec^-1</t>
+  </si>
+  <si>
+    <t>Performance breadth (Tbr)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pringleophaga </t>
+  </si>
+  <si>
+    <t>marioni</t>
+  </si>
+  <si>
+    <t>Figure 1</t>
+  </si>
+  <si>
+    <t>Thermal preference</t>
+  </si>
+  <si>
+    <t>excluding CTmin</t>
+  </si>
+  <si>
+    <t>including CTmin</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
 </sst>
 </file>
 
@@ -769,11 +808,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FD9C74-7293-0D4C-AEEE-5123D41AED94}">
-  <dimension ref="A1:AH303"/>
+  <dimension ref="A1:AH318"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A285" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M302" sqref="M302:M303"/>
+      <pane ySplit="1" topLeftCell="A296" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H319" sqref="H319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24073,6 +24112,1152 @@
         <v>125</v>
       </c>
     </row>
+    <row r="304" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A304" s="1">
+        <v>1</v>
+      </c>
+      <c r="B304" s="1">
+        <v>1</v>
+      </c>
+      <c r="C304" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D304" t="s">
+        <v>129</v>
+      </c>
+      <c r="E304" s="1">
+        <v>0</v>
+      </c>
+      <c r="F304" s="1">
+        <v>1</v>
+      </c>
+      <c r="H304" s="1">
+        <v>10</v>
+      </c>
+      <c r="I304" s="1">
+        <v>10</v>
+      </c>
+      <c r="J304" s="1">
+        <v>24</v>
+      </c>
+      <c r="K304" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L304" t="s">
+        <v>43</v>
+      </c>
+      <c r="M304">
+        <v>23.6</v>
+      </c>
+      <c r="N304">
+        <v>22.9</v>
+      </c>
+      <c r="O304">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="P304">
+        <v>0.79</v>
+      </c>
+      <c r="Q304" s="1">
+        <v>35</v>
+      </c>
+      <c r="R304" s="1">
+        <v>33</v>
+      </c>
+      <c r="S304" s="1">
+        <v>0</v>
+      </c>
+      <c r="T304" s="1">
+        <v>0</v>
+      </c>
+      <c r="U304" t="s">
+        <v>132</v>
+      </c>
+      <c r="V304" t="s">
+        <v>133</v>
+      </c>
+      <c r="W304" s="1">
+        <v>1</v>
+      </c>
+      <c r="X304" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y304" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="305" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A305" s="1">
+        <v>2</v>
+      </c>
+      <c r="B305" s="1">
+        <v>1</v>
+      </c>
+      <c r="C305" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D305" t="s">
+        <v>129</v>
+      </c>
+      <c r="E305" s="1">
+        <v>0</v>
+      </c>
+      <c r="F305" s="1">
+        <v>1</v>
+      </c>
+      <c r="H305" s="1">
+        <v>10</v>
+      </c>
+      <c r="I305" s="1">
+        <v>10</v>
+      </c>
+      <c r="J305" s="1">
+        <v>24</v>
+      </c>
+      <c r="K305" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L305" t="s">
+        <v>130</v>
+      </c>
+      <c r="M305">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="N305">
+        <v>5.4</v>
+      </c>
+      <c r="O305">
+        <v>0.25</v>
+      </c>
+      <c r="P305">
+        <v>0.22</v>
+      </c>
+      <c r="Q305" s="1">
+        <v>28</v>
+      </c>
+      <c r="R305" s="1">
+        <v>28</v>
+      </c>
+      <c r="S305" s="1">
+        <v>0</v>
+      </c>
+      <c r="T305" s="1">
+        <v>0</v>
+      </c>
+      <c r="U305" t="s">
+        <v>132</v>
+      </c>
+      <c r="V305" t="s">
+        <v>133</v>
+      </c>
+      <c r="W305" s="1">
+        <v>1</v>
+      </c>
+      <c r="X305" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y305" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="306" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A306" s="1">
+        <v>3</v>
+      </c>
+      <c r="B306" s="1">
+        <v>1</v>
+      </c>
+      <c r="C306" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D306" t="s">
+        <v>129</v>
+      </c>
+      <c r="E306" s="1">
+        <v>0</v>
+      </c>
+      <c r="F306" s="1">
+        <v>1</v>
+      </c>
+      <c r="H306" s="1">
+        <v>10</v>
+      </c>
+      <c r="I306" s="1">
+        <v>10</v>
+      </c>
+      <c r="J306" s="1">
+        <v>24</v>
+      </c>
+      <c r="K306" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="L306" t="s">
+        <v>43</v>
+      </c>
+      <c r="M306">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="N306">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="O306">
+        <v>0.92</v>
+      </c>
+      <c r="P306">
+        <v>0.77</v>
+      </c>
+      <c r="Q306" s="1">
+        <v>35</v>
+      </c>
+      <c r="R306" s="1">
+        <v>33</v>
+      </c>
+      <c r="S306" s="1">
+        <v>0</v>
+      </c>
+      <c r="T306" s="1">
+        <v>0</v>
+      </c>
+      <c r="U306" t="s">
+        <v>132</v>
+      </c>
+      <c r="V306" t="s">
+        <v>133</v>
+      </c>
+      <c r="W306" s="1">
+        <v>1</v>
+      </c>
+      <c r="X306" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y306" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="307" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A307" s="1">
+        <v>1</v>
+      </c>
+      <c r="B307" s="1">
+        <v>2</v>
+      </c>
+      <c r="C307" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D307" t="s">
+        <v>134</v>
+      </c>
+      <c r="E307" s="1">
+        <v>0</v>
+      </c>
+      <c r="F307" s="1">
+        <v>1</v>
+      </c>
+      <c r="H307" s="1">
+        <v>10</v>
+      </c>
+      <c r="I307" s="1">
+        <v>10</v>
+      </c>
+      <c r="J307" s="1">
+        <v>24</v>
+      </c>
+      <c r="K307" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="L307" t="s">
+        <v>43</v>
+      </c>
+      <c r="M307">
+        <v>8.0827067669172799</v>
+      </c>
+      <c r="N307">
+        <v>4.5422674303772297</v>
+      </c>
+      <c r="O307">
+        <v>9.1200222779170144</v>
+      </c>
+      <c r="P307">
+        <v>3.4004871946803705</v>
+      </c>
+      <c r="Q307" s="1">
+        <v>35</v>
+      </c>
+      <c r="R307" s="1">
+        <v>33</v>
+      </c>
+      <c r="S307" s="1">
+        <v>1</v>
+      </c>
+      <c r="T307" s="1">
+        <v>1</v>
+      </c>
+      <c r="U307" t="s">
+        <v>132</v>
+      </c>
+      <c r="V307" t="s">
+        <v>133</v>
+      </c>
+      <c r="W307" s="1">
+        <v>1</v>
+      </c>
+      <c r="X307" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y307" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA307" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="308" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A308" s="1">
+        <v>1</v>
+      </c>
+      <c r="B308" s="1">
+        <v>2</v>
+      </c>
+      <c r="C308" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D308" t="s">
+        <v>134</v>
+      </c>
+      <c r="E308" s="1">
+        <v>0</v>
+      </c>
+      <c r="F308" s="1">
+        <v>1</v>
+      </c>
+      <c r="H308" s="1">
+        <v>10</v>
+      </c>
+      <c r="I308" s="1">
+        <v>10</v>
+      </c>
+      <c r="J308" s="1">
+        <v>24</v>
+      </c>
+      <c r="K308" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="L308" t="s">
+        <v>43</v>
+      </c>
+      <c r="M308">
+        <v>5.3571428571428399</v>
+      </c>
+      <c r="N308">
+        <v>3.9689907169662302</v>
+      </c>
+      <c r="O308">
+        <v>9.8858256752993263</v>
+      </c>
+      <c r="P308">
+        <v>4.7358834244080077</v>
+      </c>
+      <c r="Q308" s="1">
+        <v>35</v>
+      </c>
+      <c r="R308" s="1">
+        <v>33</v>
+      </c>
+      <c r="S308" s="1">
+        <v>1</v>
+      </c>
+      <c r="T308" s="1">
+        <v>1</v>
+      </c>
+      <c r="U308" t="s">
+        <v>132</v>
+      </c>
+      <c r="V308" t="s">
+        <v>133</v>
+      </c>
+      <c r="W308" s="1">
+        <v>1</v>
+      </c>
+      <c r="X308" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y308" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA308" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="309" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A309" s="1">
+        <v>1</v>
+      </c>
+      <c r="B309" s="1">
+        <v>3</v>
+      </c>
+      <c r="C309" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D309" t="s">
+        <v>55</v>
+      </c>
+      <c r="E309" s="1">
+        <v>0</v>
+      </c>
+      <c r="F309" s="1">
+        <v>1</v>
+      </c>
+      <c r="H309" s="1">
+        <v>10</v>
+      </c>
+      <c r="I309" s="1">
+        <v>10</v>
+      </c>
+      <c r="J309" s="1">
+        <v>24</v>
+      </c>
+      <c r="K309" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L309" t="s">
+        <v>43</v>
+      </c>
+      <c r="M309">
+        <v>22.794117647058801</v>
+      </c>
+      <c r="N309">
+        <v>22.509559599156098</v>
+      </c>
+      <c r="O309">
+        <v>5.6644880174291838</v>
+      </c>
+      <c r="P309">
+        <v>3.8287232380059248</v>
+      </c>
+      <c r="Q309" s="1">
+        <v>35</v>
+      </c>
+      <c r="R309" s="1">
+        <v>33</v>
+      </c>
+      <c r="S309" s="1">
+        <v>1</v>
+      </c>
+      <c r="T309" s="1">
+        <v>1</v>
+      </c>
+      <c r="U309" t="s">
+        <v>132</v>
+      </c>
+      <c r="V309" t="s">
+        <v>133</v>
+      </c>
+      <c r="W309" s="1">
+        <v>1</v>
+      </c>
+      <c r="X309" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y309" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA309" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="310" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A310" s="1">
+        <v>1</v>
+      </c>
+      <c r="B310" s="1">
+        <v>3</v>
+      </c>
+      <c r="C310" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D310" t="s">
+        <v>55</v>
+      </c>
+      <c r="E310" s="1">
+        <v>0</v>
+      </c>
+      <c r="F310" s="1">
+        <v>1</v>
+      </c>
+      <c r="H310" s="1">
+        <v>10</v>
+      </c>
+      <c r="I310" s="1">
+        <v>10</v>
+      </c>
+      <c r="J310" s="1">
+        <v>24</v>
+      </c>
+      <c r="K310" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L310" t="s">
+        <v>43</v>
+      </c>
+      <c r="M310">
+        <v>5.4411764705881804</v>
+      </c>
+      <c r="N310">
+        <v>5.0857067510549401</v>
+      </c>
+      <c r="O310">
+        <v>9.8039215686273806</v>
+      </c>
+      <c r="P310">
+        <v>10.172609978121592</v>
+      </c>
+      <c r="Q310" s="1">
+        <v>35</v>
+      </c>
+      <c r="R310" s="1">
+        <v>33</v>
+      </c>
+      <c r="S310" s="1">
+        <v>1</v>
+      </c>
+      <c r="T310" s="1">
+        <v>1</v>
+      </c>
+      <c r="U310" t="s">
+        <v>132</v>
+      </c>
+      <c r="V310" t="s">
+        <v>133</v>
+      </c>
+      <c r="W310" s="1">
+        <v>1</v>
+      </c>
+      <c r="X310" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y310" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA310" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="311" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A311" s="1">
+        <v>1</v>
+      </c>
+      <c r="B311" s="1">
+        <v>4</v>
+      </c>
+      <c r="C311" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D311" t="s">
+        <v>81</v>
+      </c>
+      <c r="E311" s="1">
+        <v>0</v>
+      </c>
+      <c r="F311" s="1">
+        <v>1</v>
+      </c>
+      <c r="G311" s="2">
+        <v>0</v>
+      </c>
+      <c r="H311" s="1">
+        <v>10</v>
+      </c>
+      <c r="I311" s="1">
+        <v>10</v>
+      </c>
+      <c r="J311" s="1">
+        <v>24</v>
+      </c>
+      <c r="K311" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L311" t="s">
+        <v>130</v>
+      </c>
+      <c r="M311">
+        <v>0.69012178619756703</v>
+      </c>
+      <c r="N311">
+        <v>0.60060060060060005</v>
+      </c>
+      <c r="O311">
+        <v>6.7658998646820012E-2</v>
+      </c>
+      <c r="P311">
+        <v>6.7567567567568487E-2</v>
+      </c>
+      <c r="Q311" s="1">
+        <v>28</v>
+      </c>
+      <c r="R311" s="1">
+        <v>28</v>
+      </c>
+      <c r="S311" s="1">
+        <v>0</v>
+      </c>
+      <c r="T311" s="1">
+        <v>0</v>
+      </c>
+      <c r="U311" t="s">
+        <v>132</v>
+      </c>
+      <c r="V311" t="s">
+        <v>133</v>
+      </c>
+      <c r="W311" s="1">
+        <v>1</v>
+      </c>
+      <c r="X311" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y311" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="312" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A312" s="1">
+        <v>1</v>
+      </c>
+      <c r="B312" s="1">
+        <v>4</v>
+      </c>
+      <c r="C312" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D312" t="s">
+        <v>81</v>
+      </c>
+      <c r="E312" s="1">
+        <v>0</v>
+      </c>
+      <c r="F312" s="1">
+        <v>1</v>
+      </c>
+      <c r="G312" s="2">
+        <v>0</v>
+      </c>
+      <c r="H312" s="1">
+        <v>10</v>
+      </c>
+      <c r="I312" s="1">
+        <v>10</v>
+      </c>
+      <c r="J312" s="1">
+        <v>24</v>
+      </c>
+      <c r="K312" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L312" t="s">
+        <v>130</v>
+      </c>
+      <c r="M312">
+        <v>1.7456021650879501</v>
+      </c>
+      <c r="N312">
+        <v>1.7867867867867799</v>
+      </c>
+      <c r="O312">
+        <v>8.1190798376185036E-2</v>
+      </c>
+      <c r="P312">
+        <v>9.0090090090090058E-2</v>
+      </c>
+      <c r="Q312" s="1">
+        <v>28</v>
+      </c>
+      <c r="R312" s="1">
+        <v>28</v>
+      </c>
+      <c r="S312" s="1">
+        <v>0</v>
+      </c>
+      <c r="T312" s="1">
+        <v>0</v>
+      </c>
+      <c r="U312" t="s">
+        <v>132</v>
+      </c>
+      <c r="V312" t="s">
+        <v>133</v>
+      </c>
+      <c r="W312" s="1">
+        <v>1</v>
+      </c>
+      <c r="X312" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y312" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A313" s="1">
+        <v>1</v>
+      </c>
+      <c r="B313" s="1">
+        <v>4</v>
+      </c>
+      <c r="C313" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D313" t="s">
+        <v>81</v>
+      </c>
+      <c r="E313" s="1">
+        <v>0</v>
+      </c>
+      <c r="F313" s="1">
+        <v>1</v>
+      </c>
+      <c r="G313" s="2">
+        <v>10.0159574468085</v>
+      </c>
+      <c r="H313" s="1">
+        <v>10</v>
+      </c>
+      <c r="I313" s="1">
+        <v>10</v>
+      </c>
+      <c r="J313" s="1">
+        <v>24</v>
+      </c>
+      <c r="K313" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L313" t="s">
+        <v>130</v>
+      </c>
+      <c r="M313">
+        <v>2.6251691474966101</v>
+      </c>
+      <c r="N313">
+        <v>2.9429429429429401</v>
+      </c>
+      <c r="O313">
+        <v>0.14884979702300516</v>
+      </c>
+      <c r="P313">
+        <v>0.16516516516516511</v>
+      </c>
+      <c r="Q313" s="1">
+        <v>28</v>
+      </c>
+      <c r="R313" s="1">
+        <v>28</v>
+      </c>
+      <c r="S313" s="1">
+        <v>0</v>
+      </c>
+      <c r="T313" s="1">
+        <v>0</v>
+      </c>
+      <c r="U313" t="s">
+        <v>132</v>
+      </c>
+      <c r="V313" t="s">
+        <v>133</v>
+      </c>
+      <c r="W313" s="1">
+        <v>1</v>
+      </c>
+      <c r="X313" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y313" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="314" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A314" s="1">
+        <v>1</v>
+      </c>
+      <c r="B314" s="1">
+        <v>4</v>
+      </c>
+      <c r="C314" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D314" t="s">
+        <v>81</v>
+      </c>
+      <c r="E314" s="1">
+        <v>0</v>
+      </c>
+      <c r="F314" s="1">
+        <v>1</v>
+      </c>
+      <c r="G314" s="2">
+        <v>15.005319148936101</v>
+      </c>
+      <c r="H314" s="1">
+        <v>10</v>
+      </c>
+      <c r="I314" s="1">
+        <v>10</v>
+      </c>
+      <c r="J314" s="1">
+        <v>24</v>
+      </c>
+      <c r="K314" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L314" t="s">
+        <v>130</v>
+      </c>
+      <c r="M314">
+        <v>3.7212449255751001</v>
+      </c>
+      <c r="N314">
+        <v>4.08408408408408</v>
+      </c>
+      <c r="O314">
+        <v>0.23004059539918997</v>
+      </c>
+      <c r="P314">
+        <v>0.1951951951951898</v>
+      </c>
+      <c r="Q314" s="1">
+        <v>28</v>
+      </c>
+      <c r="R314" s="1">
+        <v>28</v>
+      </c>
+      <c r="S314" s="1">
+        <v>0</v>
+      </c>
+      <c r="T314" s="1">
+        <v>0</v>
+      </c>
+      <c r="U314" t="s">
+        <v>132</v>
+      </c>
+      <c r="V314" t="s">
+        <v>133</v>
+      </c>
+      <c r="W314" s="1">
+        <v>1</v>
+      </c>
+      <c r="X314" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y314" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="315" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A315" s="1">
+        <v>1</v>
+      </c>
+      <c r="B315" s="1">
+        <v>4</v>
+      </c>
+      <c r="C315" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D315" t="s">
+        <v>81</v>
+      </c>
+      <c r="E315" s="1">
+        <v>0</v>
+      </c>
+      <c r="F315" s="1">
+        <v>1</v>
+      </c>
+      <c r="G315" s="2">
+        <v>19.994680851063801</v>
+      </c>
+      <c r="H315" s="1">
+        <v>10</v>
+      </c>
+      <c r="I315" s="1">
+        <v>10</v>
+      </c>
+      <c r="J315" s="1">
+        <v>24</v>
+      </c>
+      <c r="K315" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L315" t="s">
+        <v>130</v>
+      </c>
+      <c r="M315">
+        <v>4.4113667117726596</v>
+      </c>
+      <c r="N315">
+        <v>4.8648648648648596</v>
+      </c>
+      <c r="O315">
+        <v>0.24357239512855466</v>
+      </c>
+      <c r="P315">
+        <v>0.21021021021020969</v>
+      </c>
+      <c r="Q315" s="1">
+        <v>28</v>
+      </c>
+      <c r="R315" s="1">
+        <v>28</v>
+      </c>
+      <c r="S315" s="1">
+        <v>0</v>
+      </c>
+      <c r="T315" s="1">
+        <v>0</v>
+      </c>
+      <c r="U315" t="s">
+        <v>132</v>
+      </c>
+      <c r="V315" t="s">
+        <v>133</v>
+      </c>
+      <c r="W315" s="1">
+        <v>1</v>
+      </c>
+      <c r="X315" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y315" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="316" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A316" s="1">
+        <v>1</v>
+      </c>
+      <c r="B316" s="1">
+        <v>4</v>
+      </c>
+      <c r="C316" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D316" t="s">
+        <v>81</v>
+      </c>
+      <c r="E316" s="1">
+        <v>0</v>
+      </c>
+      <c r="F316" s="1">
+        <v>1</v>
+      </c>
+      <c r="G316" s="2">
+        <v>24.984042553191401</v>
+      </c>
+      <c r="H316" s="1">
+        <v>10</v>
+      </c>
+      <c r="I316" s="1">
+        <v>10</v>
+      </c>
+      <c r="J316" s="1">
+        <v>24</v>
+      </c>
+      <c r="K316" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L316" t="s">
+        <v>130</v>
+      </c>
+      <c r="M316">
+        <v>4.2489851150202904</v>
+      </c>
+      <c r="N316">
+        <v>4.8048048048048004</v>
+      </c>
+      <c r="O316">
+        <v>0.30446549391068989</v>
+      </c>
+      <c r="P316">
+        <v>0.247747747747745</v>
+      </c>
+      <c r="Q316" s="1">
+        <v>28</v>
+      </c>
+      <c r="R316" s="1">
+        <v>28</v>
+      </c>
+      <c r="S316" s="1">
+        <v>0</v>
+      </c>
+      <c r="T316" s="1">
+        <v>0</v>
+      </c>
+      <c r="U316" t="s">
+        <v>132</v>
+      </c>
+      <c r="V316" t="s">
+        <v>133</v>
+      </c>
+      <c r="W316" s="1">
+        <v>1</v>
+      </c>
+      <c r="X316" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y316" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="317" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A317" s="1">
+        <v>1</v>
+      </c>
+      <c r="B317" s="1">
+        <v>4</v>
+      </c>
+      <c r="C317" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D317" t="s">
+        <v>81</v>
+      </c>
+      <c r="E317" s="1">
+        <v>0</v>
+      </c>
+      <c r="F317" s="1">
+        <v>1</v>
+      </c>
+      <c r="G317" s="2">
+        <v>30.010638297872301</v>
+      </c>
+      <c r="H317" s="1">
+        <v>10</v>
+      </c>
+      <c r="I317" s="1">
+        <v>10</v>
+      </c>
+      <c r="J317" s="1">
+        <v>24</v>
+      </c>
+      <c r="K317" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L317" t="s">
+        <v>130</v>
+      </c>
+      <c r="M317">
+        <v>4.04600811907983</v>
+      </c>
+      <c r="N317">
+        <v>3.97897897897897</v>
+      </c>
+      <c r="O317">
+        <v>0.28416779431664496</v>
+      </c>
+      <c r="P317">
+        <v>0.16516516516516511</v>
+      </c>
+      <c r="Q317" s="1">
+        <v>28</v>
+      </c>
+      <c r="R317" s="1">
+        <v>28</v>
+      </c>
+      <c r="S317" s="1">
+        <v>0</v>
+      </c>
+      <c r="T317" s="1">
+        <v>0</v>
+      </c>
+      <c r="U317" t="s">
+        <v>132</v>
+      </c>
+      <c r="V317" t="s">
+        <v>133</v>
+      </c>
+      <c r="W317" s="1">
+        <v>1</v>
+      </c>
+      <c r="X317" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y317" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="318" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A318" s="1">
+        <v>1</v>
+      </c>
+      <c r="B318" s="1">
+        <v>4</v>
+      </c>
+      <c r="C318" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D318" t="s">
+        <v>81</v>
+      </c>
+      <c r="E318" s="1">
+        <v>0</v>
+      </c>
+      <c r="F318" s="1">
+        <v>1</v>
+      </c>
+      <c r="G318" s="2">
+        <v>34.999999999999901</v>
+      </c>
+      <c r="H318" s="1">
+        <v>10</v>
+      </c>
+      <c r="I318" s="1">
+        <v>10</v>
+      </c>
+      <c r="J318" s="1">
+        <v>24</v>
+      </c>
+      <c r="K318" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L318" t="s">
+        <v>130</v>
+      </c>
+      <c r="M318">
+        <v>3.3152909336941798</v>
+      </c>
+      <c r="N318">
+        <v>3.2132132132132099</v>
+      </c>
+      <c r="O318">
+        <v>0.21650879566981995</v>
+      </c>
+      <c r="P318">
+        <v>0.22522522522522492</v>
+      </c>
+      <c r="Q318" s="1">
+        <v>28</v>
+      </c>
+      <c r="R318" s="1">
+        <v>28</v>
+      </c>
+      <c r="S318" s="1">
+        <v>0</v>
+      </c>
+      <c r="T318" s="1">
+        <v>0</v>
+      </c>
+      <c r="U318" t="s">
+        <v>132</v>
+      </c>
+      <c r="V318" t="s">
+        <v>133</v>
+      </c>
+      <c r="W318" s="1">
+        <v>1</v>
+      </c>
+      <c r="X318" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y318" s="1">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
peng et al 2014, completing the acclimation data extraction
</commit_message>
<xml_diff>
--- a/data extraction /extraction /acclimation /data/acclimation_full_2june21.xlsx
+++ b/data extraction /extraction /acclimation /data/acclimation_full_2june21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /extraction /acclimation /data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60ADDCA2-C131-8146-958B-C81FB0CCCB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE13309-2AFD-DB4B-B78E-6B2625080D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29420" yWindow="-24160" windowWidth="23500" windowHeight="12900" xr2:uid="{BC548A7C-C40E-CC48-BA60-2918C3D37144}"/>
+    <workbookView xWindow="5300" yWindow="860" windowWidth="23500" windowHeight="12900" xr2:uid="{BC548A7C-C40E-CC48-BA60-2918C3D37144}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2024" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2082" uniqueCount="155">
   <si>
     <t>response_id</t>
   </si>
@@ -443,6 +443,54 @@
   <si>
     <t>Speed</t>
   </si>
+  <si>
+    <t>maneti2018</t>
+  </si>
+  <si>
+    <t>exposure environment</t>
+  </si>
+  <si>
+    <t>fluctuating</t>
+  </si>
+  <si>
+    <t>constant</t>
+  </si>
+  <si>
+    <t>Time to heat knockdown</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>simulans</t>
+  </si>
+  <si>
+    <t>peng2014</t>
+  </si>
+  <si>
+    <t>Figure 1a</t>
+  </si>
+  <si>
+    <t>Figure 1b</t>
+  </si>
+  <si>
+    <t>Figure 1c</t>
+  </si>
+  <si>
+    <t>Figure 1d</t>
+  </si>
+  <si>
+    <t>LTmax</t>
+  </si>
+  <si>
+    <t>LTmin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parabramis </t>
+  </si>
+  <si>
+    <t>pekinensis</t>
+  </si>
 </sst>
 </file>
 
@@ -808,11 +856,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FD9C74-7293-0D4C-AEEE-5123D41AED94}">
-  <dimension ref="A1:AH318"/>
+  <dimension ref="A1:AH327"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A296" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H319" sqref="H319"/>
+      <pane ySplit="1" topLeftCell="A307" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T329" sqref="T329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24698,7 +24746,7 @@
         <v>28</v>
       </c>
       <c r="S311" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T311" s="1">
         <v>0</v>
@@ -24775,7 +24823,7 @@
         <v>28</v>
       </c>
       <c r="S312" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T312" s="1">
         <v>0</v>
@@ -24852,7 +24900,7 @@
         <v>28</v>
       </c>
       <c r="S313" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T313" s="1">
         <v>0</v>
@@ -24929,7 +24977,7 @@
         <v>28</v>
       </c>
       <c r="S314" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T314" s="1">
         <v>0</v>
@@ -25006,7 +25054,7 @@
         <v>28</v>
       </c>
       <c r="S315" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T315" s="1">
         <v>0</v>
@@ -25083,7 +25131,7 @@
         <v>28</v>
       </c>
       <c r="S316" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T316" s="1">
         <v>0</v>
@@ -25160,7 +25208,7 @@
         <v>28</v>
       </c>
       <c r="S317" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T317" s="1">
         <v>0</v>
@@ -25237,7 +25285,7 @@
         <v>28</v>
       </c>
       <c r="S318" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T318" s="1">
         <v>0</v>
@@ -25256,6 +25304,690 @@
       </c>
       <c r="Y318" s="1">
         <v>1</v>
+      </c>
+      <c r="Z318" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA318" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="319" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A319" s="1">
+        <v>1</v>
+      </c>
+      <c r="B319" s="1">
+        <v>1</v>
+      </c>
+      <c r="C319" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D319" t="s">
+        <v>134</v>
+      </c>
+      <c r="E319" s="1">
+        <v>0</v>
+      </c>
+      <c r="F319" s="1">
+        <v>1</v>
+      </c>
+      <c r="G319" s="2">
+        <v>37.5</v>
+      </c>
+      <c r="H319" s="1">
+        <v>23</v>
+      </c>
+      <c r="I319" s="1">
+        <v>15</v>
+      </c>
+      <c r="J319" s="1">
+        <v>24</v>
+      </c>
+      <c r="K319" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="L319" t="s">
+        <v>144</v>
+      </c>
+      <c r="M319" s="3">
+        <v>61.776134300000002</v>
+      </c>
+      <c r="N319" s="3">
+        <v>58.528296699999999</v>
+      </c>
+      <c r="O319">
+        <v>1.7616221999999999</v>
+      </c>
+      <c r="P319">
+        <v>2.2107081200000001</v>
+      </c>
+      <c r="Q319" s="1">
+        <v>192</v>
+      </c>
+      <c r="R319" s="1">
+        <v>192</v>
+      </c>
+      <c r="S319" s="1">
+        <v>1</v>
+      </c>
+      <c r="T319" s="1">
+        <v>0</v>
+      </c>
+      <c r="U319" t="s">
+        <v>115</v>
+      </c>
+      <c r="V319" t="s">
+        <v>145</v>
+      </c>
+      <c r="W319" s="1">
+        <v>1</v>
+      </c>
+      <c r="X319" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y319" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z319" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA319" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="320" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A320" s="1">
+        <v>1</v>
+      </c>
+      <c r="B320" s="1">
+        <v>2</v>
+      </c>
+      <c r="C320" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D320" t="s">
+        <v>134</v>
+      </c>
+      <c r="E320" s="1">
+        <v>0</v>
+      </c>
+      <c r="F320" s="1">
+        <v>1</v>
+      </c>
+      <c r="G320" s="2">
+        <v>37.5</v>
+      </c>
+      <c r="H320" s="1">
+        <v>23</v>
+      </c>
+      <c r="I320" s="1">
+        <v>15</v>
+      </c>
+      <c r="J320" s="1">
+        <v>24</v>
+      </c>
+      <c r="K320" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="L320" t="s">
+        <v>144</v>
+      </c>
+      <c r="M320" s="3">
+        <v>36.0766524</v>
+      </c>
+      <c r="N320" s="3">
+        <v>29.7198633</v>
+      </c>
+      <c r="O320">
+        <v>1.8307426600000001</v>
+      </c>
+      <c r="P320">
+        <v>1.51986183</v>
+      </c>
+      <c r="Q320" s="1">
+        <v>192</v>
+      </c>
+      <c r="R320" s="1">
+        <v>192</v>
+      </c>
+      <c r="S320" s="1">
+        <v>1</v>
+      </c>
+      <c r="T320" s="1">
+        <v>0</v>
+      </c>
+      <c r="U320" t="s">
+        <v>115</v>
+      </c>
+      <c r="V320" t="s">
+        <v>145</v>
+      </c>
+      <c r="W320" s="1">
+        <v>1</v>
+      </c>
+      <c r="X320" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y320" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="321" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A321" s="1">
+        <v>1</v>
+      </c>
+      <c r="B321" s="1">
+        <v>3</v>
+      </c>
+      <c r="C321" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D321" t="s">
+        <v>74</v>
+      </c>
+      <c r="E321" s="1">
+        <v>0</v>
+      </c>
+      <c r="F321" s="1">
+        <v>1</v>
+      </c>
+      <c r="H321" s="1">
+        <v>23</v>
+      </c>
+      <c r="I321" s="1">
+        <v>15</v>
+      </c>
+      <c r="J321" s="1">
+        <v>24</v>
+      </c>
+      <c r="K321" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L321" t="s">
+        <v>144</v>
+      </c>
+      <c r="M321">
+        <v>39.054339116499399</v>
+      </c>
+      <c r="N321">
+        <v>40.230621169999999</v>
+      </c>
+      <c r="O321" s="3">
+        <v>0.11858974</v>
+      </c>
+      <c r="P321">
+        <v>9.6153846153850253E-2</v>
+      </c>
+      <c r="Q321" s="1">
+        <v>16</v>
+      </c>
+      <c r="R321" s="1">
+        <v>16</v>
+      </c>
+      <c r="S321" s="1">
+        <v>1</v>
+      </c>
+      <c r="T321" s="1">
+        <v>0</v>
+      </c>
+      <c r="U321" t="s">
+        <v>115</v>
+      </c>
+      <c r="V321" t="s">
+        <v>145</v>
+      </c>
+      <c r="W321" s="1">
+        <v>1</v>
+      </c>
+      <c r="X321" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y321" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="322" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A322" s="1">
+        <v>1</v>
+      </c>
+      <c r="B322" s="1">
+        <v>3</v>
+      </c>
+      <c r="C322" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D322" t="s">
+        <v>74</v>
+      </c>
+      <c r="E322" s="1">
+        <v>0</v>
+      </c>
+      <c r="F322" s="1">
+        <v>1</v>
+      </c>
+      <c r="H322" s="1">
+        <v>23</v>
+      </c>
+      <c r="I322" s="1">
+        <v>15</v>
+      </c>
+      <c r="J322" s="1">
+        <v>24</v>
+      </c>
+      <c r="K322" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L322" t="s">
+        <v>144</v>
+      </c>
+      <c r="M322">
+        <v>39.445207984949803</v>
+      </c>
+      <c r="N322">
+        <v>39.852259267001102</v>
+      </c>
+      <c r="O322">
+        <v>0.10576923076919797</v>
+      </c>
+      <c r="P322">
+        <v>8.1730769230752287E-2</v>
+      </c>
+      <c r="Q322" s="1">
+        <v>16</v>
+      </c>
+      <c r="R322" s="1">
+        <v>16</v>
+      </c>
+      <c r="S322" s="1">
+        <v>1</v>
+      </c>
+      <c r="T322" s="1">
+        <v>0</v>
+      </c>
+      <c r="U322" t="s">
+        <v>115</v>
+      </c>
+      <c r="V322" t="s">
+        <v>145</v>
+      </c>
+      <c r="W322" s="1">
+        <v>1</v>
+      </c>
+      <c r="X322" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y322" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="323" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A323" s="1">
+        <v>1</v>
+      </c>
+      <c r="B323" s="1">
+        <v>3</v>
+      </c>
+      <c r="C323" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D323" t="s">
+        <v>74</v>
+      </c>
+      <c r="E323" s="1">
+        <v>0</v>
+      </c>
+      <c r="F323" s="1">
+        <v>1</v>
+      </c>
+      <c r="H323" s="1">
+        <v>23</v>
+      </c>
+      <c r="I323" s="1">
+        <v>15</v>
+      </c>
+      <c r="J323" s="1">
+        <v>24</v>
+      </c>
+      <c r="K323" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L323" t="s">
+        <v>144</v>
+      </c>
+      <c r="M323">
+        <v>39.637358904682202</v>
+      </c>
+      <c r="N323">
+        <v>40.005948648272003</v>
+      </c>
+      <c r="O323">
+        <v>0.11858974358970187</v>
+      </c>
+      <c r="P323">
+        <v>6.8914611204000664E-2</v>
+      </c>
+      <c r="Q323" s="1">
+        <v>16</v>
+      </c>
+      <c r="R323" s="1">
+        <v>16</v>
+      </c>
+      <c r="S323" s="1">
+        <v>1</v>
+      </c>
+      <c r="T323" s="1">
+        <v>0</v>
+      </c>
+      <c r="U323" t="s">
+        <v>115</v>
+      </c>
+      <c r="V323" t="s">
+        <v>145</v>
+      </c>
+      <c r="W323" s="1">
+        <v>1</v>
+      </c>
+      <c r="X323" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y323" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="324" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A324" s="1">
+        <v>1</v>
+      </c>
+      <c r="B324" s="1">
+        <v>1</v>
+      </c>
+      <c r="C324" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D324" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E324" s="1">
+        <v>0</v>
+      </c>
+      <c r="F324" s="1">
+        <v>1</v>
+      </c>
+      <c r="H324" s="1">
+        <v>20</v>
+      </c>
+      <c r="I324" s="1">
+        <v>10</v>
+      </c>
+      <c r="J324" s="1">
+        <v>24</v>
+      </c>
+      <c r="K324" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L324" t="s">
+        <v>43</v>
+      </c>
+      <c r="M324" s="3">
+        <v>33.283018900000002</v>
+      </c>
+      <c r="N324" s="3">
+        <v>35.264150899999997</v>
+      </c>
+      <c r="O324">
+        <v>0.79245283</v>
+      </c>
+      <c r="P324">
+        <v>0.59433961999999996</v>
+      </c>
+      <c r="Q324" s="1">
+        <v>8</v>
+      </c>
+      <c r="R324" s="1">
+        <v>8</v>
+      </c>
+      <c r="S324" s="1">
+        <v>1</v>
+      </c>
+      <c r="T324" s="1">
+        <v>0</v>
+      </c>
+      <c r="U324" t="s">
+        <v>153</v>
+      </c>
+      <c r="V324" t="s">
+        <v>154</v>
+      </c>
+      <c r="W324" s="1">
+        <v>1</v>
+      </c>
+      <c r="X324" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y324" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="325" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A325" s="1">
+        <v>2</v>
+      </c>
+      <c r="B325" s="1">
+        <v>1</v>
+      </c>
+      <c r="C325" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D325" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E325" s="1">
+        <v>0</v>
+      </c>
+      <c r="F325" s="1">
+        <v>1</v>
+      </c>
+      <c r="H325" s="1">
+        <v>20</v>
+      </c>
+      <c r="I325" s="1">
+        <v>10</v>
+      </c>
+      <c r="J325" s="1">
+        <v>24</v>
+      </c>
+      <c r="K325" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L325" t="s">
+        <v>43</v>
+      </c>
+      <c r="M325" s="3">
+        <v>5.1844155799999996</v>
+      </c>
+      <c r="N325" s="3">
+        <v>4.8772517799999999</v>
+      </c>
+      <c r="O325">
+        <v>0.25345622000000001</v>
+      </c>
+      <c r="P325">
+        <v>0.18433179999999999</v>
+      </c>
+      <c r="Q325" s="1">
+        <v>8</v>
+      </c>
+      <c r="R325" s="1">
+        <v>8</v>
+      </c>
+      <c r="S325" s="1">
+        <v>1</v>
+      </c>
+      <c r="T325" s="1">
+        <v>0</v>
+      </c>
+      <c r="U325" t="s">
+        <v>153</v>
+      </c>
+      <c r="V325" t="s">
+        <v>154</v>
+      </c>
+      <c r="W325" s="1">
+        <v>1</v>
+      </c>
+      <c r="X325" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y325" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="326" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A326" s="1">
+        <v>3</v>
+      </c>
+      <c r="B326" s="1">
+        <v>1</v>
+      </c>
+      <c r="C326" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D326" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E326" s="1">
+        <v>0</v>
+      </c>
+      <c r="F326" s="1">
+        <v>1</v>
+      </c>
+      <c r="H326" s="1">
+        <v>20</v>
+      </c>
+      <c r="I326" s="1">
+        <v>10</v>
+      </c>
+      <c r="J326" s="1">
+        <v>24</v>
+      </c>
+      <c r="K326" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="L326" t="s">
+        <v>43</v>
+      </c>
+      <c r="M326" s="3">
+        <v>34.194690299999998</v>
+      </c>
+      <c r="N326">
+        <v>36.053097299999997</v>
+      </c>
+      <c r="O326">
+        <v>0.37168141999999998</v>
+      </c>
+      <c r="P326">
+        <v>0.18584070999999999</v>
+      </c>
+      <c r="Q326" s="1">
+        <v>8</v>
+      </c>
+      <c r="R326" s="1">
+        <v>8</v>
+      </c>
+      <c r="S326" s="1">
+        <v>1</v>
+      </c>
+      <c r="T326" s="1">
+        <v>0</v>
+      </c>
+      <c r="U326" t="s">
+        <v>153</v>
+      </c>
+      <c r="V326" t="s">
+        <v>154</v>
+      </c>
+      <c r="W326" s="1">
+        <v>1</v>
+      </c>
+      <c r="X326" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y326" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="327" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A327" s="1">
+        <v>4</v>
+      </c>
+      <c r="B327" s="1">
+        <v>1</v>
+      </c>
+      <c r="C327" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D327" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E327" s="1">
+        <v>0</v>
+      </c>
+      <c r="F327" s="1">
+        <v>1</v>
+      </c>
+      <c r="H327" s="1">
+        <v>20</v>
+      </c>
+      <c r="I327" s="1">
+        <v>10</v>
+      </c>
+      <c r="J327" s="1">
+        <v>24</v>
+      </c>
+      <c r="K327" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="L327" t="s">
+        <v>43</v>
+      </c>
+      <c r="M327" s="3">
+        <v>3.4199134199999999</v>
+      </c>
+      <c r="N327" s="3">
+        <v>2.5541125500000001</v>
+      </c>
+      <c r="O327">
+        <v>0.19480518999999999</v>
+      </c>
+      <c r="P327">
+        <v>0.17316017</v>
+      </c>
+      <c r="Q327" s="1">
+        <v>8</v>
+      </c>
+      <c r="R327" s="1">
+        <v>8</v>
+      </c>
+      <c r="S327" s="1">
+        <v>1</v>
+      </c>
+      <c r="T327" s="1">
+        <v>0</v>
+      </c>
+      <c r="U327" t="s">
+        <v>153</v>
+      </c>
+      <c r="V327" t="s">
+        <v>154</v>
+      </c>
+      <c r="W327" s="1">
+        <v>1</v>
+      </c>
+      <c r="X327" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y327" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sheldon et al extraction for acclimation analysis
</commit_message>
<xml_diff>
--- a/data extraction /extraction /acclimation /data/acclimation_full_2june21.xlsx
+++ b/data extraction /extraction /acclimation /data/acclimation_full_2june21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /extraction /acclimation /data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE13309-2AFD-DB4B-B78E-6B2625080D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BE36B9-5371-6846-AB11-39D037CE4663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5300" yWindow="860" windowWidth="23500" windowHeight="12900" xr2:uid="{BC548A7C-C40E-CC48-BA60-2918C3D37144}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2082" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2130" uniqueCount="160">
   <si>
     <t>response_id</t>
   </si>
@@ -491,6 +491,21 @@
   <si>
     <t>pekinensis</t>
   </si>
+  <si>
+    <t>sheldon2020</t>
+  </si>
+  <si>
+    <t>log CO2 production</t>
+  </si>
+  <si>
+    <t>uL * min^-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phanaeus </t>
+  </si>
+  <si>
+    <t>vindex</t>
+  </si>
 </sst>
 </file>
 
@@ -856,11 +871,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FD9C74-7293-0D4C-AEEE-5123D41AED94}">
-  <dimension ref="A1:AH327"/>
+  <dimension ref="A1:AH335"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A307" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T329" sqref="T329"/>
+      <pane ySplit="1" topLeftCell="A318" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P332" sqref="P332:P335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25990,6 +26005,622 @@
         <v>2</v>
       </c>
     </row>
+    <row r="328" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A328" s="1">
+        <v>1</v>
+      </c>
+      <c r="B328" s="1">
+        <v>1</v>
+      </c>
+      <c r="C328" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D328" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E328" s="1">
+        <v>0</v>
+      </c>
+      <c r="F328" s="1">
+        <v>0</v>
+      </c>
+      <c r="G328" s="5">
+        <v>9.9925458767404205</v>
+      </c>
+      <c r="H328" s="1">
+        <v>20</v>
+      </c>
+      <c r="I328" s="1">
+        <v>5</v>
+      </c>
+      <c r="J328" s="1">
+        <v>24</v>
+      </c>
+      <c r="K328" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="L328" t="s">
+        <v>157</v>
+      </c>
+      <c r="M328">
+        <v>0.46273932253313699</v>
+      </c>
+      <c r="N328">
+        <v>0.44653902798232697</v>
+      </c>
+      <c r="O328">
+        <v>6.774668630338751E-2</v>
+      </c>
+      <c r="P328">
+        <v>6.4064801178202985E-2</v>
+      </c>
+      <c r="Q328" s="1">
+        <v>5</v>
+      </c>
+      <c r="R328" s="1">
+        <v>5</v>
+      </c>
+      <c r="S328" s="1">
+        <v>1</v>
+      </c>
+      <c r="T328" s="1">
+        <v>0</v>
+      </c>
+      <c r="U328" t="s">
+        <v>158</v>
+      </c>
+      <c r="V328" t="s">
+        <v>159</v>
+      </c>
+      <c r="W328" s="3">
+        <v>1</v>
+      </c>
+      <c r="X328" s="3">
+        <v>2</v>
+      </c>
+      <c r="Y328" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="329" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A329" s="1">
+        <v>1</v>
+      </c>
+      <c r="B329" s="1">
+        <v>1</v>
+      </c>
+      <c r="C329" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D329" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E329" s="1">
+        <v>0</v>
+      </c>
+      <c r="F329" s="1">
+        <v>0</v>
+      </c>
+      <c r="G329" s="5">
+        <v>15.005308239290899</v>
+      </c>
+      <c r="H329" s="1">
+        <v>20</v>
+      </c>
+      <c r="I329" s="1">
+        <v>5</v>
+      </c>
+      <c r="J329" s="1">
+        <v>24</v>
+      </c>
+      <c r="K329" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="L329" t="s">
+        <v>157</v>
+      </c>
+      <c r="M329">
+        <v>0.51870397643593502</v>
+      </c>
+      <c r="N329">
+        <v>0.41413843888070601</v>
+      </c>
+      <c r="O329">
+        <v>6.4801178203239995E-2</v>
+      </c>
+      <c r="P329">
+        <v>7.0692194403534497E-2</v>
+      </c>
+      <c r="Q329" s="1">
+        <v>5</v>
+      </c>
+      <c r="R329" s="1">
+        <v>5</v>
+      </c>
+      <c r="S329" s="1">
+        <v>1</v>
+      </c>
+      <c r="T329" s="1">
+        <v>0</v>
+      </c>
+      <c r="U329" t="s">
+        <v>158</v>
+      </c>
+      <c r="V329" t="s">
+        <v>159</v>
+      </c>
+      <c r="W329" s="3">
+        <v>1</v>
+      </c>
+      <c r="X329" s="3">
+        <v>2</v>
+      </c>
+      <c r="Y329" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="330" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A330" s="1">
+        <v>1</v>
+      </c>
+      <c r="B330" s="1">
+        <v>1</v>
+      </c>
+      <c r="C330" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D330" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E330" s="1">
+        <v>0</v>
+      </c>
+      <c r="F330" s="1">
+        <v>0</v>
+      </c>
+      <c r="G330" s="5">
+        <v>20.014275775454699</v>
+      </c>
+      <c r="H330" s="1">
+        <v>20</v>
+      </c>
+      <c r="I330" s="1">
+        <v>5</v>
+      </c>
+      <c r="J330" s="1">
+        <v>24</v>
+      </c>
+      <c r="K330" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="L330" t="s">
+        <v>157</v>
+      </c>
+      <c r="M330">
+        <v>0.65714285714285703</v>
+      </c>
+      <c r="N330">
+        <v>0.54226804123711303</v>
+      </c>
+      <c r="O330">
+        <v>8.5419734904271016E-2</v>
+      </c>
+      <c r="P330">
+        <v>9.2783505154639484E-2</v>
+      </c>
+      <c r="Q330" s="1">
+        <v>5</v>
+      </c>
+      <c r="R330" s="1">
+        <v>5</v>
+      </c>
+      <c r="S330" s="1">
+        <v>1</v>
+      </c>
+      <c r="T330" s="1">
+        <v>0</v>
+      </c>
+      <c r="U330" t="s">
+        <v>158</v>
+      </c>
+      <c r="V330" t="s">
+        <v>159</v>
+      </c>
+      <c r="W330" s="3">
+        <v>1</v>
+      </c>
+      <c r="X330" s="3">
+        <v>2</v>
+      </c>
+      <c r="Y330" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="331" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A331" s="1">
+        <v>1</v>
+      </c>
+      <c r="B331" s="1">
+        <v>1</v>
+      </c>
+      <c r="C331" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D331" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E331" s="1">
+        <v>0</v>
+      </c>
+      <c r="F331" s="1">
+        <v>0</v>
+      </c>
+      <c r="G331" s="5">
+        <v>24.985328930129999</v>
+      </c>
+      <c r="H331" s="1">
+        <v>20</v>
+      </c>
+      <c r="I331" s="1">
+        <v>5</v>
+      </c>
+      <c r="J331" s="1">
+        <v>24</v>
+      </c>
+      <c r="K331" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="L331" t="s">
+        <v>157</v>
+      </c>
+      <c r="M331">
+        <v>0.61958762886597896</v>
+      </c>
+      <c r="N331">
+        <v>0.62326951399116304</v>
+      </c>
+      <c r="O331">
+        <v>8.2474226804124029E-2</v>
+      </c>
+      <c r="P331">
+        <v>8.61561119293075E-2</v>
+      </c>
+      <c r="Q331" s="1">
+        <v>5</v>
+      </c>
+      <c r="R331" s="1">
+        <v>5</v>
+      </c>
+      <c r="S331" s="1">
+        <v>1</v>
+      </c>
+      <c r="T331" s="1">
+        <v>0</v>
+      </c>
+      <c r="U331" t="s">
+        <v>158</v>
+      </c>
+      <c r="V331" t="s">
+        <v>159</v>
+      </c>
+      <c r="W331" s="3">
+        <v>1</v>
+      </c>
+      <c r="X331" s="3">
+        <v>2</v>
+      </c>
+      <c r="Y331" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="332" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A332" s="1">
+        <v>1</v>
+      </c>
+      <c r="B332" s="1">
+        <v>1</v>
+      </c>
+      <c r="C332" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D332" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E332" s="1">
+        <v>0</v>
+      </c>
+      <c r="F332" s="1">
+        <v>0</v>
+      </c>
+      <c r="G332" s="5">
+        <v>9.9925458767404205</v>
+      </c>
+      <c r="H332" s="1">
+        <v>20</v>
+      </c>
+      <c r="I332" s="1">
+        <v>12</v>
+      </c>
+      <c r="J332" s="1">
+        <v>24</v>
+      </c>
+      <c r="K332" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="L332" t="s">
+        <v>157</v>
+      </c>
+      <c r="M332">
+        <v>0.46273932253313699</v>
+      </c>
+      <c r="N332">
+        <v>0.44653902798232697</v>
+      </c>
+      <c r="O332">
+        <v>6.774668630338751E-2</v>
+      </c>
+      <c r="P332">
+        <v>6.6273932253313989E-2</v>
+      </c>
+      <c r="Q332" s="1">
+        <v>5</v>
+      </c>
+      <c r="R332" s="1">
+        <v>5</v>
+      </c>
+      <c r="S332" s="1">
+        <v>1</v>
+      </c>
+      <c r="T332" s="1">
+        <v>0</v>
+      </c>
+      <c r="U332" t="s">
+        <v>158</v>
+      </c>
+      <c r="V332" t="s">
+        <v>159</v>
+      </c>
+      <c r="W332" s="3">
+        <v>1</v>
+      </c>
+      <c r="X332" s="3">
+        <v>2</v>
+      </c>
+      <c r="Y332" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="333" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A333" s="1">
+        <v>1</v>
+      </c>
+      <c r="B333" s="1">
+        <v>1</v>
+      </c>
+      <c r="C333" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D333" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E333" s="1">
+        <v>0</v>
+      </c>
+      <c r="F333" s="1">
+        <v>0</v>
+      </c>
+      <c r="G333" s="5">
+        <v>15.005308239290899</v>
+      </c>
+      <c r="H333" s="1">
+        <v>20</v>
+      </c>
+      <c r="I333" s="1">
+        <v>12</v>
+      </c>
+      <c r="J333" s="1">
+        <v>24</v>
+      </c>
+      <c r="K333" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="L333" t="s">
+        <v>157</v>
+      </c>
+      <c r="M333">
+        <v>0.51870397643593502</v>
+      </c>
+      <c r="N333">
+        <v>0.48335787923416701</v>
+      </c>
+      <c r="O333">
+        <v>6.4801178203239995E-2</v>
+      </c>
+      <c r="P333">
+        <v>7.2164948453608463E-2</v>
+      </c>
+      <c r="Q333" s="1">
+        <v>5</v>
+      </c>
+      <c r="R333" s="1">
+        <v>5</v>
+      </c>
+      <c r="S333" s="1">
+        <v>1</v>
+      </c>
+      <c r="T333" s="1">
+        <v>0</v>
+      </c>
+      <c r="U333" t="s">
+        <v>158</v>
+      </c>
+      <c r="V333" t="s">
+        <v>159</v>
+      </c>
+      <c r="W333" s="3">
+        <v>1</v>
+      </c>
+      <c r="X333" s="3">
+        <v>2</v>
+      </c>
+      <c r="Y333" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="334" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A334" s="1">
+        <v>1</v>
+      </c>
+      <c r="B334" s="1">
+        <v>1</v>
+      </c>
+      <c r="C334" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D334" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E334" s="1">
+        <v>0</v>
+      </c>
+      <c r="F334" s="1">
+        <v>0</v>
+      </c>
+      <c r="G334" s="5">
+        <v>20.014275775454699</v>
+      </c>
+      <c r="H334" s="1">
+        <v>20</v>
+      </c>
+      <c r="I334" s="1">
+        <v>12</v>
+      </c>
+      <c r="J334" s="1">
+        <v>24</v>
+      </c>
+      <c r="K334" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="L334" t="s">
+        <v>157</v>
+      </c>
+      <c r="M334">
+        <v>0.65714285714285703</v>
+      </c>
+      <c r="N334">
+        <v>0.57172312223858601</v>
+      </c>
+      <c r="O334">
+        <v>8.5419734904271016E-2</v>
+      </c>
+      <c r="P334">
+        <v>7.2901325478644974E-2</v>
+      </c>
+      <c r="Q334" s="1">
+        <v>5</v>
+      </c>
+      <c r="R334" s="1">
+        <v>5</v>
+      </c>
+      <c r="S334" s="1">
+        <v>1</v>
+      </c>
+      <c r="T334" s="1">
+        <v>0</v>
+      </c>
+      <c r="U334" t="s">
+        <v>158</v>
+      </c>
+      <c r="V334" t="s">
+        <v>159</v>
+      </c>
+      <c r="W334" s="3">
+        <v>1</v>
+      </c>
+      <c r="X334" s="3">
+        <v>2</v>
+      </c>
+      <c r="Y334" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="335" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A335" s="1">
+        <v>1</v>
+      </c>
+      <c r="B335" s="1">
+        <v>1</v>
+      </c>
+      <c r="C335" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D335" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E335" s="1">
+        <v>0</v>
+      </c>
+      <c r="F335" s="1">
+        <v>0</v>
+      </c>
+      <c r="G335" s="5">
+        <v>24.985328930129999</v>
+      </c>
+      <c r="H335" s="1">
+        <v>20</v>
+      </c>
+      <c r="I335" s="1">
+        <v>12</v>
+      </c>
+      <c r="J335" s="1">
+        <v>24</v>
+      </c>
+      <c r="K335" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="L335" t="s">
+        <v>157</v>
+      </c>
+      <c r="M335">
+        <v>0.61958762886597896</v>
+      </c>
+      <c r="N335">
+        <v>0.57319587628865898</v>
+      </c>
+      <c r="O335">
+        <v>8.2474226804124029E-2</v>
+      </c>
+      <c r="P335">
+        <v>8.2474226804124001E-2</v>
+      </c>
+      <c r="Q335" s="1">
+        <v>5</v>
+      </c>
+      <c r="R335" s="1">
+        <v>5</v>
+      </c>
+      <c r="S335" s="1">
+        <v>1</v>
+      </c>
+      <c r="T335" s="1">
+        <v>0</v>
+      </c>
+      <c r="U335" t="s">
+        <v>158</v>
+      </c>
+      <c r="V335" t="s">
+        <v>159</v>
+      </c>
+      <c r="W335" s="3">
+        <v>1</v>
+      </c>
+      <c r="X335" s="3">
+        <v>2</v>
+      </c>
+      <c r="Y335" s="3">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>